<commit_message>
Comentarios y correcion de un peño bug
</commit_message>
<xml_diff>
--- a/Newton_Raphson.xlsx
+++ b/Newton_Raphson.xlsx
@@ -411,7 +411,7 @@
         <v>-5.479999999999997</v>
       </c>
       <c r="E2">
-        <v>-0.1469781021897809</v>
+        <v>1.546978102189781</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -431,7 +431,7 @@
         <v>-1.949132857259374</v>
       </c>
       <c r="E3">
-        <v>52.01208211648346</v>
+        <v>1.559853335846044</v>
       </c>
       <c r="F3">
         <v>1.194230656934307</v>
@@ -451,7 +451,7 @@
         <v>-3.305981176598917</v>
       </c>
       <c r="E4">
-        <v>10.28139172134779</v>
+        <v>1.560040640984931</v>
       </c>
       <c r="F4">
         <v>0.394746463626362</v>
@@ -471,7 +471,7 @@
         <v>-4.337509072011899</v>
       </c>
       <c r="E5">
-        <v>1.928347920314901</v>
+        <v>1.560040682404453</v>
       </c>
       <c r="F5">
         <v>0.2450892408724875</v>
@@ -491,7 +491,7 @@
         <v>-3.813224177742161</v>
       </c>
       <c r="E6">
-        <v>-0.097903249551827</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F6">
         <v>0.1200594067667623</v>
@@ -511,7 +511,7 @@
         <v>-4.14119756942833</v>
       </c>
       <c r="E7">
-        <v>-19.28209750781475</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F7">
         <v>0.0756354362618531</v>
@@ -531,7 +531,7 @@
         <v>-3.945833182250865</v>
       </c>
       <c r="E8">
-        <v>-3.974513340249296</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F8">
         <v>0.04473042572167274</v>
@@ -551,7 +551,7 @@
         <v>-4.066869380529078</v>
       </c>
       <c r="E9">
-        <v>-0.9076935257401058</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F9">
         <v>0.02780054156410583</v>
@@ -571,7 +571,7 @@
         <v>-3.993320219045278</v>
       </c>
       <c r="E10">
-        <v>-0.01899446287468407</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F10">
         <v>0.01685357827800071</v>
@@ -591,7 +591,7 @@
         <v>-4.038609391048757</v>
       </c>
       <c r="E11">
-        <v>-6.817570098865597</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F11">
         <v>0.01039119798028798</v>
@@ -611,7 +611,7 @@
         <v>-4.010931113843964</v>
       </c>
       <c r="E12">
-        <v>-1.479608397757289</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F12">
         <v>0.006345173426217876</v>
@@ -631,7 +631,7 @@
         <v>-4.027928324779606</v>
       </c>
       <c r="E13">
-        <v>-0.3348495467935433</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F13">
         <v>0.003898496746425284</v>
@@ -651,7 +651,7 @@
         <v>-4.017520321626253</v>
       </c>
       <c r="E14">
-        <v>2.30837857080335</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F14">
         <v>0.002386445182463892</v>
@@ -671,7 +671,7 @@
         <v>-4.023904946889688</v>
       </c>
       <c r="E15">
-        <v>0.1808794491614419</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F15">
         <v>0.001464202450720653</v>
@@ -691,7 +691,7 @@
         <v>-4.019992655665443</v>
       </c>
       <c r="E16">
-        <v>-3.089554001385319</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F16">
         <v>0.0008971112736644304</v>
@@ -711,7 +711,7 @@
         <v>-4.022391589282584</v>
       </c>
       <c r="E17">
-        <v>-0.7261009231790462</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F17">
         <v>0.0005501285468370032</v>
@@ -731,7 +731,7 @@
         <v>-4.020921216691302</v>
       </c>
       <c r="E18">
-        <v>0.2101678755619217</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F18">
         <v>0.0003371742409884471</v>
@@ -751,7 +751,7 @@
         <v>-4.021822675466277</v>
       </c>
       <c r="E19">
-        <v>-2.890275785442197</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F19">
         <v>0.0002067209332328179</v>
@@ -771,7 +771,7 @@
         <v>-4.021270092576946</v>
       </c>
       <c r="E20">
-        <v>-0.6842869918365811</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F20">
         <v>0.0001267152544893735</v>
@@ -791,7 +791,7 @@
         <v>-4.021608850957852</v>
       </c>
       <c r="E21">
-        <v>0.2863075648321038</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F21">
         <v>7.768297979127148E-05</v>
@@ -811,7 +811,7 @@
         <v>-4.021401188728992</v>
       </c>
       <c r="E22">
-        <v>-2.477390443266051</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F22">
         <v>4.762013959258571E-05</v>
@@ -831,7 +831,7 @@
         <v>-4.021528492244832</v>
       </c>
       <c r="E23">
-        <v>-0.5953012680143811</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F23">
         <v>2.919276223634082E-05</v>
@@ -851,7 +851,7 @@
         <v>-4.021450452861052</v>
       </c>
       <c r="E24">
-        <v>0.4985808778160221</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F24">
         <v>1.789565582122066E-05</v>
@@ -871,7 +871,7 @@
         <v>-4.02149829306923</v>
       </c>
       <c r="E25">
-        <v>-1.695772873770362</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F25">
         <v>1.097052632614837E-05</v>
@@ -891,7 +891,7 @@
         <v>-4.021468965995069</v>
       </c>
       <c r="E26">
-        <v>-0.403139993193902</v>
+        <v>1.560040682404455</v>
       </c>
       <c r="F26">
         <v>6.725162194132217E-06</v>

</xml_diff>